<commit_message>
Update code and datasets
Upload datasets from clean data folder, upload descriptive statistics notebook
</commit_message>
<xml_diff>
--- a/data/data management sheet.xlsx
+++ b/data/data management sheet.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29530"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://lsecloud-my.sharepoint.com/personal/a_jaremko_lse_ac_uk/Documents/YEAR 2/PP4V8 - policy paper/policy-paper-repo/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://lsecloud-my.sharepoint.com/personal/a_jaremko_lse_ac_uk/Documents/YEAR 2/1. Policy paper/policy-paper-repo/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="71" documentId="11_F25DC773A252ABDACC10482B211E79645BDE58F1" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{9C343273-D391-4CCE-9E68-28CDEA688FFE}"/>
+  <xr:revisionPtr revIDLastSave="127" documentId="11_F25DC773A252ABDACC10482B211E79645BDE58F1" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{99BA379E-3BDC-4889-90DA-DBABAC50719A}"/>
   <bookViews>
-    <workbookView xWindow="-4335" yWindow="8002" windowWidth="21795" windowHeight="12975" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-4095" yWindow="8002" windowWidth="21795" windowHeight="12975" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Outcome" sheetId="2" r:id="rId1"/>
@@ -18,17 +18,28 @@
     <sheet name="Matching" sheetId="4" r:id="rId3"/>
     <sheet name="Control" sheetId="5" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="28">
   <si>
     <t>variable_name</t>
   </si>
@@ -58,16 +69,84 @@
   </si>
   <si>
     <t>index</t>
+  </si>
+  <si>
+    <t>description</t>
+  </si>
+  <si>
+    <t>Bank Danych Lokalnych (GUS</t>
+  </si>
+  <si>
+    <t>NUTS-3</t>
+  </si>
+  <si>
+    <t>Poland</t>
+  </si>
+  <si>
+    <t>link to folder</t>
+  </si>
+  <si>
+    <t>year_min</t>
+  </si>
+  <si>
+    <t>year_max</t>
+  </si>
+  <si>
+    <t>frequency</t>
+  </si>
+  <si>
+    <t>annual</t>
+  </si>
+  <si>
+    <t>Gross domestic product per capita</t>
+  </si>
+  <si>
+    <t>Gross domestic product per capita, Poland=100</t>
+  </si>
+  <si>
+    <t>Gross domestic product per capita, region=100</t>
+  </si>
+  <si>
+    <t>NUTS-4</t>
+  </si>
+  <si>
+    <t>NUTS-5</t>
+  </si>
+  <si>
+    <t>link to source</t>
+  </si>
+  <si>
+    <t>EU</t>
+  </si>
+  <si>
+    <t>Geofiles</t>
+  </si>
+  <si>
+    <t>EUROSTAT</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -90,16 +169,27 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="1">
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -174,18 +264,21 @@
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{E09BF70B-F031-42DA-8302-3893B37DEF16}" name="Table26" displayName="Table26" ref="A1:J8" totalsRowShown="0">
-  <autoFilter ref="A1:J8" xr:uid="{E09BF70B-F031-42DA-8302-3893B37DEF16}"/>
-  <tableColumns count="10">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{E09BF70B-F031-42DA-8302-3893B37DEF16}" name="Table26" displayName="Table26" ref="A1:M8" totalsRowShown="0">
+  <autoFilter ref="A1:M8" xr:uid="{E09BF70B-F031-42DA-8302-3893B37DEF16}"/>
+  <tableColumns count="13">
     <tableColumn id="1" xr3:uid="{FF10C0DC-D318-4657-8BC1-936456612C36}" name="index"/>
     <tableColumn id="2" xr3:uid="{998ABEF2-22A3-4FC1-AD88-C80BBAEBED36}" name="source"/>
     <tableColumn id="3" xr3:uid="{F390DF03-2410-444B-B216-04B327C7E967}" name="citation_doi"/>
     <tableColumn id="4" xr3:uid="{094B74C0-D3EC-46B7-9209-8E94F902650D}" name="var_code"/>
     <tableColumn id="5" xr3:uid="{9EEE37A0-83CF-4CB5-BE7A-6265677CB4BC}" name="variable_name"/>
-    <tableColumn id="6" xr3:uid="{317B1903-4989-47B6-A1C1-85BC3CA9474E}" name="drive_link"/>
-    <tableColumn id="7" xr3:uid="{7FDC3EA5-1818-4553-B554-A6AF5A73C91C}" name="year_coverage"/>
+    <tableColumn id="12" xr3:uid="{2526D3E6-AA5C-43B7-A823-7B3E4A0BE34A}" name="description" dataDxfId="0"/>
+    <tableColumn id="6" xr3:uid="{6E7EFCE9-4DA0-4190-9F1D-6D0D3756FED0}" name="year_min"/>
+    <tableColumn id="11" xr3:uid="{6B57EE3E-AA23-4A28-A10D-6F525519CFB2}" name="year_max"/>
+    <tableColumn id="7" xr3:uid="{7FDC3EA5-1818-4553-B554-A6AF5A73C91C}" name="frequency"/>
     <tableColumn id="8" xr3:uid="{9DB49739-37FA-4D2B-BFEF-56D0E11178DD}" name="granularity"/>
     <tableColumn id="9" xr3:uid="{E71AA0B1-FB18-4C46-AEAC-6889C7F3CA23}" name="country_coverage"/>
+    <tableColumn id="13" xr3:uid="{9F4E5164-249F-4E7B-9B3E-90C478AA7EEA}" name="drive_link"/>
     <tableColumn id="10" xr3:uid="{480D5735-B598-4C2E-9FD9-F89162EA1C83}" name="notes"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight21" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -461,19 +554,19 @@
       <selection sqref="A1:J8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.59765625" customWidth="1"/>
-    <col min="3" max="3" width="19.06640625" customWidth="1"/>
-    <col min="4" max="4" width="9.73046875" customWidth="1"/>
-    <col min="5" max="5" width="20.33203125" customWidth="1"/>
-    <col min="6" max="6" width="13.06640625" customWidth="1"/>
-    <col min="7" max="7" width="15.6640625" customWidth="1"/>
+    <col min="1" max="1" width="9.5703125" customWidth="1"/>
+    <col min="3" max="3" width="19" customWidth="1"/>
+    <col min="4" max="4" width="9.7109375" customWidth="1"/>
+    <col min="5" max="5" width="20.28515625" customWidth="1"/>
+    <col min="6" max="6" width="13" customWidth="1"/>
+    <col min="7" max="7" width="15.7109375" customWidth="1"/>
     <col min="8" max="8" width="19" customWidth="1"/>
-    <col min="9" max="9" width="16.59765625" customWidth="1"/>
+    <col min="9" max="9" width="16.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>9</v>
       </c>
@@ -505,17 +598,17 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
@@ -536,9 +629,9 @@
       <selection sqref="A1:J8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>9</v>
       </c>
@@ -570,17 +663,17 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
@@ -601,9 +694,9 @@
       <selection sqref="A1:J8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>9</v>
       </c>
@@ -635,17 +728,17 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
@@ -660,25 +753,29 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3E26B436-D73A-4BFA-A853-AAFBE9ADE270}">
-  <dimension ref="A1:J4"/>
+  <dimension ref="A1:M8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J22" sqref="J22"/>
+    <sheetView tabSelected="1" zoomScale="110" workbookViewId="0">
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="14.19921875" customWidth="1"/>
-    <col min="3" max="3" width="12.59765625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.59765625" customWidth="1"/>
-    <col min="5" max="5" width="17.265625" customWidth="1"/>
-    <col min="6" max="7" width="18.6640625" customWidth="1"/>
-    <col min="8" max="8" width="16.19921875" customWidth="1"/>
-    <col min="9" max="9" width="18.1328125" customWidth="1"/>
-    <col min="10" max="10" width="16.796875" customWidth="1"/>
+    <col min="1" max="1" width="6" customWidth="1"/>
+    <col min="2" max="2" width="26.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.5703125" customWidth="1"/>
+    <col min="5" max="5" width="17.28515625" customWidth="1"/>
+    <col min="6" max="6" width="15.85546875" style="3" customWidth="1"/>
+    <col min="7" max="7" width="18.42578125" customWidth="1"/>
+    <col min="8" max="8" width="17.28515625" customWidth="1"/>
+    <col min="9" max="9" width="18.7109375" customWidth="1"/>
+    <col min="10" max="10" width="16.140625" customWidth="1"/>
+    <col min="11" max="12" width="18.140625" customWidth="1"/>
+    <col min="13" max="13" width="16.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>9</v>
       </c>
@@ -694,41 +791,176 @@
       <c r="E1" t="s">
         <v>0</v>
       </c>
-      <c r="F1" t="s">
+      <c r="F1" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="G1" t="s">
+        <v>15</v>
+      </c>
+      <c r="H1" t="s">
+        <v>16</v>
+      </c>
+      <c r="I1" t="s">
+        <v>17</v>
+      </c>
+      <c r="J1" t="s">
+        <v>3</v>
+      </c>
+      <c r="K1" t="s">
+        <v>4</v>
+      </c>
+      <c r="L1" t="s">
         <v>1</v>
       </c>
-      <c r="G1" t="s">
-        <v>2</v>
-      </c>
-      <c r="H1" t="s">
-        <v>3</v>
-      </c>
-      <c r="I1" t="s">
-        <v>4</v>
-      </c>
-      <c r="J1" t="s">
+      <c r="M1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="B2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="G2">
+        <v>2000</v>
+      </c>
+      <c r="H2">
+        <v>2023</v>
+      </c>
+      <c r="I2" t="s">
+        <v>18</v>
+      </c>
+      <c r="J2" t="s">
+        <v>12</v>
+      </c>
+      <c r="K2" t="s">
+        <v>13</v>
+      </c>
+      <c r="L2" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="B3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="F3" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="G3">
+        <v>2000</v>
+      </c>
+      <c r="H3">
+        <v>2023</v>
+      </c>
+      <c r="I3" t="s">
+        <v>18</v>
+      </c>
+      <c r="J3" t="s">
+        <v>22</v>
+      </c>
+      <c r="K3" t="s">
+        <v>13</v>
+      </c>
+      <c r="L3" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
+      <c r="B4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="F4" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="G4">
+        <v>2000</v>
+      </c>
+      <c r="H4">
+        <v>2023</v>
+      </c>
+      <c r="I4" t="s">
+        <v>18</v>
+      </c>
+      <c r="J4" t="s">
+        <v>23</v>
+      </c>
+      <c r="K4" t="s">
+        <v>13</v>
+      </c>
+      <c r="L4" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5" t="s">
+        <v>27</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="F5" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="H5">
+        <v>2024</v>
+      </c>
+      <c r="J5" t="s">
+        <v>12</v>
+      </c>
+      <c r="K5" t="s">
+        <v>25</v>
+      </c>
+      <c r="L5" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="F6" s="2"/>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="F7" s="2"/>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="F8" s="2"/>
     </row>
   </sheetData>
+  <phoneticPr fontId="2" type="noConversion"/>
+  <hyperlinks>
+    <hyperlink ref="L2" r:id="rId1" xr:uid="{AFCF3790-281F-4729-A638-95EBF1170BAA}"/>
+    <hyperlink ref="L3" r:id="rId2" xr:uid="{6F12C47B-83FC-4949-8066-5129B3919F96}"/>
+    <hyperlink ref="L4" r:id="rId3" xr:uid="{1DA539C4-7ADA-462A-BE49-5AF0702D3580}"/>
+    <hyperlink ref="C2" r:id="rId4" xr:uid="{3D4B9407-ED3A-4A86-ACC9-FAEBC9CB8077}"/>
+    <hyperlink ref="C3:C4" r:id="rId5" display="link to source" xr:uid="{7B34B539-5B6A-4E51-ABA6-904D8C4E409A}"/>
+    <hyperlink ref="L5" r:id="rId6" xr:uid="{1F5FAD2F-68C2-47BB-83AD-187278957596}"/>
+    <hyperlink ref="C5" r:id="rId7" xr:uid="{7D836333-49D1-4298-9CA4-5E509FB01B37}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="1">
-    <tablePart r:id="rId1"/>
+    <tablePart r:id="rId8"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>